<commit_message>
adding files to server pressing changes to date_log
</commit_message>
<xml_diff>
--- a/Database Code/db_example.xlsx
+++ b/Database Code/db_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="password" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>emp_id</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>ui/ux</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Thrs</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
   </si>
 </sst>
 </file>
@@ -150,21 +165,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -732,10 +768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D1"/>
+  <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -743,7 +779,7 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:11">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -753,9 +789,245 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11">
+      <c r="B2">
+        <v>1001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42467</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42467</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4">
+        <v>1003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42467</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5">
+        <v>1004</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42467</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6">
+        <v>1005</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42467</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7">
+        <v>1001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42468</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8">
+        <v>1002</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42468</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9">
+        <v>1003</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42468</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10">
+        <v>1004</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42468</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11">
+        <v>1005</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42468</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12">
+        <v>1001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42471</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13">
+        <v>1002</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42471</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14">
+        <v>1003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42471</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15">
+        <v>1004</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42471</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16">
+        <v>1005</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42471</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17">
+        <v>1001</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42472</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18">
+        <v>1002</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42472</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19">
+        <v>1003</v>
+      </c>
+      <c r="C19" s="1">
+        <v>42472</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20">
+        <v>1004</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42472</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21">
+        <v>1005</v>
+      </c>
+      <c r="C21" s="1">
+        <v>42472</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>